<commit_message>
Take Home Assignment 4 File
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Google Drive (sanaa.rafique@utexas.edu)\LBJ School of Public Affairs\Spring 2019\Data Management with Python\Take Home Assignment 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
   <si>
     <t>Variable Name</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Sector</t>
   </si>
   <si>
-    <t>ZIP</t>
-  </si>
-  <si>
-    <t>ZIP Code of Instiution</t>
-  </si>
-  <si>
     <t>Longitude</t>
   </si>
   <si>
@@ -252,6 +246,63 @@
   </si>
   <si>
     <t>Poverty Rate of Institution's ZIP Code in 2012</t>
+  </si>
+  <si>
+    <t>ZIP_NEW</t>
+  </si>
+  <si>
+    <t>ZIP Code of Institution</t>
+  </si>
+  <si>
+    <t>Avg_enroll_W_12-17</t>
+  </si>
+  <si>
+    <t>Avg_enroll_B_12-18</t>
+  </si>
+  <si>
+    <t>Avg_enroll_H_12-19</t>
+  </si>
+  <si>
+    <t>Avg_enroll_A_12-20</t>
+  </si>
+  <si>
+    <t>Average enrollment of white students in Texas higher educational institutions between 2012 and 2017 (%)</t>
+  </si>
+  <si>
+    <t>Average enrollment of Hispanic students in Texas higher educational institutions between 2012 and 2017 (%)</t>
+  </si>
+  <si>
+    <t>Average enrollment of Asian students in Texas higher educational institutions between 2012 and 2017 (%)</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>zips</t>
+  </si>
+  <si>
+    <t>avg_povrate</t>
+  </si>
+  <si>
+    <t>Avg_enroll_12-17</t>
+  </si>
+  <si>
+    <t>Average enrollment of all students in Texas higher educational institutions between 2012 and 2017 (%)</t>
+  </si>
+  <si>
+    <t>Average enrollment of black students in Texas higher educational institutions between 2012 and 2017 (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of zipcodes which are within 6 miles of the instution's latitude and longitude coordinates. </t>
+  </si>
+  <si>
+    <t>Average poverty rate of the variable "zips" between 2012 and 2017</t>
   </si>
 </sst>
 </file>
@@ -295,10 +346,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,16 +634,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="64" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="89.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -613,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -621,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -629,274 +683,355 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
         <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all the relevant files
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Course-Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -287,9 +287,6 @@
     <t>zips</t>
   </si>
   <si>
-    <t>avg_povrate</t>
-  </si>
-  <si>
     <t>Avg_enroll_12-17</t>
   </si>
   <si>
@@ -302,7 +299,10 @@
     <t xml:space="preserve">List of zipcodes which are within 6 miles of the instution's latitude and longitude coordinates. </t>
   </si>
   <si>
-    <t>Average poverty rate of the variable "zips" between 2012 and 2017</t>
+    <t>avg_povpoprate</t>
+  </si>
+  <si>
+    <t>Average poverty rate weighted bypopulation size of the variable "zips" between 2012 and 2017</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,7 +963,7 @@
         <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -984,10 +984,10 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
         <v>88</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1019,12 +1019,12 @@
         <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
         <v>92</v>

</xml_diff>